<commit_message>
popravljen holidays exel fajl
</commit_message>
<xml_diff>
--- a/Flask_Backend/rawTrainingData/holidays/Training Data_US Holidays 2018-2021.xlsx
+++ b/Flask_Backend/rawTrainingData/holidays/Training Data_US Holidays 2018-2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhpwsbjut5lxpst6orzs49ytdkk.sharepoint.com/sites/ProductResearchandDevelopment/Shared Documents/General/Load Forecast Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marko\Desktop\Training Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9406B723-26DA-4A67-9474-4F1354E45827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A42830-13BB-47E3-9627-C2296A379550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4B055610-134E-4B13-92E8-896F5ECCFBB2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4B055610-134E-4B13-92E8-896F5ECCFBB2}"/>
   </bookViews>
   <sheets>
     <sheet name="US Holidays" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="26">
   <si>
     <t>Monday</t>
   </si>
@@ -110,6 +109,9 @@
   </si>
   <si>
     <t>Saturday</t>
+  </si>
+  <si>
+    <t>New Year's Eve</t>
   </si>
 </sst>
 </file>
@@ -117,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -274,20 +276,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -605,25 +607,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0593F234-F7F3-4803-A580-A4FB13FCD7C2}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="28.77734375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
       <c r="A1">
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1">
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
@@ -634,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -645,7 +647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1">
       <c r="B4" s="15" t="s">
         <v>3</v>
       </c>
@@ -656,7 +658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1">
       <c r="B5" s="15" t="s">
         <v>0</v>
       </c>
@@ -667,7 +669,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1">
       <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
@@ -678,7 +680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1">
       <c r="B7" s="15" t="s">
         <v>8</v>
       </c>
@@ -689,7 +691,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1">
       <c r="B8" s="15" t="s">
         <v>8</v>
       </c>
@@ -700,7 +702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1">
       <c r="B9" s="15" t="s">
         <v>0</v>
       </c>
@@ -711,7 +713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1">
       <c r="B10" s="15" t="s">
         <v>6</v>
       </c>
@@ -722,7 +724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1">
       <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
@@ -733,7 +735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1">
       <c r="B12" s="15" t="s">
         <v>3</v>
       </c>
@@ -744,7 +746,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1">
       <c r="B13" s="15" t="s">
         <v>0</v>
       </c>
@@ -755,7 +757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1">
       <c r="B14" s="15" t="s">
         <v>0</v>
       </c>
@@ -766,7 +768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1">
       <c r="B15" s="15" t="s">
         <v>3</v>
       </c>
@@ -777,7 +779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1">
       <c r="B16" s="15" t="s">
         <v>8</v>
       </c>
@@ -788,7 +790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1">
       <c r="B17" s="15" t="s">
         <v>19</v>
       </c>
@@ -799,7 +801,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1">
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
@@ -810,569 +812,613 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1">
-      <c r="A19">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="15">
+        <v>43465</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A20">
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1">
-      <c r="B20" s="7" t="s">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C21" s="15">
         <v>43466</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1">
-      <c r="B21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="13">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="13">
         <v>43486</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1">
-      <c r="B22" s="5" t="s">
+    <row r="23" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C23" s="14">
         <v>43510</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1">
-      <c r="B23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="13">
+    <row r="24" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="13">
         <v>43514</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1">
-      <c r="B24" s="5" t="s">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C25" s="14">
         <v>43574</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1">
-      <c r="B25" s="3" t="s">
+    <row r="26" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C26" s="13">
         <v>43576</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1">
-      <c r="B26" s="5" t="s">
+    <row r="27" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C27" s="14">
         <v>43597</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1">
-      <c r="B27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="13">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="13">
         <v>43612</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1">
-      <c r="B28" s="5" t="s">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B29" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C29" s="14">
         <v>43632</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1">
-      <c r="B29" s="3" t="s">
+    <row r="30" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C30" s="13">
         <v>43650</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1">
-      <c r="B30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="14">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B31" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="14">
         <v>43710</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1">
-      <c r="B31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="13">
+    <row r="32" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="13">
         <v>43752</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1">
-      <c r="B32" s="5" t="s">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C33" s="14">
         <v>43769</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1">
-      <c r="B33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="13">
+    <row r="34" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="13">
         <v>43780</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1">
-      <c r="B34" s="5" t="s">
+    <row r="35" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B35" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C35" s="14">
         <v>43797</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1">
-      <c r="B35" s="9" t="s">
+    <row r="36" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B36" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C36" s="16">
         <v>43824</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1">
-      <c r="A36">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B37" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="16">
+        <v>43830</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A38">
         <v>2020</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1">
-      <c r="B37" s="7" t="s">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B39" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C39" s="15">
         <v>43831</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1">
-      <c r="B38" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="13">
+    <row r="40" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="13">
         <v>43850</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1">
-      <c r="B39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="14">
-        <v>43875</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1">
-      <c r="B40" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="13">
-        <v>43878</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1">
+    <row r="41" spans="1:4" ht="15.75" thickBot="1">
       <c r="B41" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="14">
+        <v>43875</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B42" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="13">
+        <v>43878</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="14">
         <v>43931</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1">
-      <c r="B42" s="3" t="s">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B44" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C44" s="13">
         <v>43933</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1">
-      <c r="B43" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="14">
-        <v>43961</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1">
-      <c r="B44" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="13">
-        <v>43976</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1">
+    <row r="45" spans="1:4" ht="15.75" thickBot="1">
       <c r="B45" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="14">
+        <v>43961</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="13">
+        <v>43976</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="14">
         <v>44003</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="29.4" thickBot="1">
-      <c r="B46" s="3" t="s">
+    <row r="48" spans="1:4" ht="30.75" thickBot="1">
+      <c r="B48" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="13">
+      <c r="C48" s="13">
         <v>44015</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1">
-      <c r="B47" s="5" t="s">
+    <row r="49" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B49" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C49" s="14">
         <v>44016</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" thickBot="1">
-      <c r="B48" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="13">
+    <row r="50" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B50" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="13">
         <v>44081</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1">
-      <c r="B49" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="14">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="14">
         <v>44116</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D51" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" thickBot="1">
-      <c r="B50" s="3" t="s">
+    <row r="52" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B52" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="13">
+      <c r="C52" s="13">
         <v>44135</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1">
-      <c r="B51" s="5" t="s">
+    <row r="53" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B53" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C53" s="14">
         <v>44146</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D53" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1">
-      <c r="B52" s="9" t="s">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B54" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="16">
+      <c r="C54" s="16">
         <v>44161</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D54" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" thickBot="1">
-      <c r="B53" s="5" t="s">
+    <row r="55" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B55" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C55" s="14">
         <v>44190</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D55" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" thickBot="1">
-      <c r="A54">
+    <row r="56" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B56" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="14">
+        <v>44186</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A57">
         <v>2021</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" thickBot="1">
-      <c r="B55" s="1" t="s">
+    <row r="58" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C55" s="12">
-        <v>43831</v>
-      </c>
-      <c r="D55" s="2" t="s">
+      <c r="C58" s="12">
+        <v>44197</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1">
-      <c r="B56" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="13">
-        <v>43850</v>
-      </c>
-      <c r="D56" s="4" t="s">
+    <row r="59" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="13">
+        <v>44216</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1">
-      <c r="B57" s="5" t="s">
+    <row r="60" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B60" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="14">
-        <v>43875</v>
-      </c>
-      <c r="D57" s="6" t="s">
+      <c r="C60" s="14">
+        <v>44241</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" thickBot="1">
-      <c r="B58" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="13">
-        <v>43878</v>
-      </c>
-      <c r="D58" s="4" t="s">
+    <row r="61" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B61" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="13">
+        <v>44244</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1">
-      <c r="B59" s="5" t="s">
+    <row r="62" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B62" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="14">
-        <v>43931</v>
-      </c>
-      <c r="D59" s="6" t="s">
+      <c r="C62" s="14">
+        <v>44296</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1">
-      <c r="B60" s="3" t="s">
+    <row r="63" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B63" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="13">
-        <v>43933</v>
-      </c>
-      <c r="D60" s="4" t="s">
+      <c r="C63" s="13">
+        <v>44298</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1">
-      <c r="B61" s="5" t="s">
+    <row r="64" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B64" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="14">
-        <v>43961</v>
-      </c>
-      <c r="D61" s="6" t="s">
+      <c r="C64" s="14">
+        <v>44326</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1">
-      <c r="B62" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C62" s="13">
-        <v>43976</v>
-      </c>
-      <c r="D62" s="4" t="s">
+    <row r="65" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B65" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="13">
+        <v>44341</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" thickBot="1">
-      <c r="B63" s="5" t="s">
+    <row r="66" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B66" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C63" s="14">
-        <v>44003</v>
-      </c>
-      <c r="D63" s="6" t="s">
+      <c r="C66" s="14">
+        <v>44368</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="29.4" thickBot="1">
-      <c r="B64" s="3" t="s">
+    <row r="67" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B67" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="13">
-        <v>44015</v>
-      </c>
-      <c r="D64" s="4" t="s">
+      <c r="C67" s="13">
+        <v>44380</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="2:4" ht="15" thickBot="1">
-      <c r="B65" s="5" t="s">
+    <row r="68" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B68" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C65" s="14">
-        <v>44016</v>
-      </c>
-      <c r="D65" s="6" t="s">
+      <c r="C68" s="14">
+        <v>44381</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="15" thickBot="1">
-      <c r="B66" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C66" s="13">
-        <v>44081</v>
-      </c>
-      <c r="D66" s="4" t="s">
+    <row r="69" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B69" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="13">
+        <v>44446</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="2:4" ht="15" thickBot="1">
-      <c r="B67" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C67" s="14">
-        <v>44116</v>
-      </c>
-      <c r="D67" s="6" t="s">
+    <row r="70" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B70" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="14">
+        <v>44481</v>
+      </c>
+      <c r="D70" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="2:4" ht="15" thickBot="1">
-      <c r="B68" s="3" t="s">
+    <row r="71" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B71" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C68" s="13">
-        <v>44135</v>
-      </c>
-      <c r="D68" s="4" t="s">
+      <c r="C71" s="13">
+        <v>44500</v>
+      </c>
+      <c r="D71" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="2:4" ht="15" thickBot="1">
-      <c r="B69" s="5" t="s">
+    <row r="72" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B72" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C69" s="14">
-        <v>44146</v>
-      </c>
-      <c r="D69" s="6" t="s">
+      <c r="C72" s="14">
+        <v>44511</v>
+      </c>
+      <c r="D72" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="2:4" ht="15" thickBot="1">
-      <c r="B70" s="3" t="s">
+    <row r="73" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B73" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C70" s="13">
-        <v>44161</v>
-      </c>
-      <c r="D70" s="4" t="s">
+      <c r="C73" s="13">
+        <v>44526</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="2:4" ht="15" thickBot="1">
-      <c r="B71" s="5" t="s">
+    <row r="74" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B74" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" s="14">
+        <v>44555</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B75" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="14">
-        <v>44190</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>22</v>
+      <c r="C75" s="14">
+        <v>44561</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1394,63 +1440,76 @@
     <hyperlink ref="D16" r:id="rId15" display="https://www.calendarlabs.com/holidays/us/veterans-day.php" xr:uid="{21CD106F-A112-4975-B2AE-373C147BF696}"/>
     <hyperlink ref="D17" r:id="rId16" display="https://www.calendarlabs.com/holidays/us/thanksgiving-day.php" xr:uid="{E04ADEEC-DE32-48B2-A4B9-F0EC00BC0589}"/>
     <hyperlink ref="D18" r:id="rId17" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{5E048B42-BD95-42FD-A22C-841EE0430751}"/>
-    <hyperlink ref="D20" r:id="rId18" display="https://www.calendarlabs.com/holidays/us/new-years-day.php" xr:uid="{0D0A3B27-3D34-4C19-B07D-9C098EEED4F4}"/>
-    <hyperlink ref="D21" r:id="rId19" display="https://www.calendarlabs.com/holidays/us/martin-luther-king-day.php" xr:uid="{4077BA1B-E655-4EC7-BD39-841A949F73AC}"/>
-    <hyperlink ref="D22" r:id="rId20" display="https://www.calendarlabs.com/holidays/us/valentines-day.php" xr:uid="{5AEF472E-5A71-4AD3-920F-81BF657457B1}"/>
-    <hyperlink ref="D23" r:id="rId21" display="https://www.calendarlabs.com/holidays/us/presidents-day.php" xr:uid="{CDFA5CE1-09BF-45C4-A38D-F7243A4DA09F}"/>
-    <hyperlink ref="D24" r:id="rId22" display="https://www.calendarlabs.com/holidays/us/good-friday.php" xr:uid="{72D2E1E7-DDAE-4B2B-8EA6-143FC11F336D}"/>
-    <hyperlink ref="D25" r:id="rId23" display="https://www.calendarlabs.com/holidays/us/easter.php" xr:uid="{ABB7BC9D-62D8-419B-A8FD-47956F4941B2}"/>
-    <hyperlink ref="D26" r:id="rId24" display="https://www.calendarlabs.com/holidays/shared/mothers-day.php" xr:uid="{E52E46E1-B1BA-4373-B2D3-4F4D2EAF98B7}"/>
-    <hyperlink ref="D27" r:id="rId25" display="https://www.calendarlabs.com/holidays/us/memorial-day.php" xr:uid="{F1D41D0A-5D96-4868-9E86-2DF5395D14A8}"/>
-    <hyperlink ref="D28" r:id="rId26" display="https://www.calendarlabs.com/holidays/shared/fathers-day.php" xr:uid="{8F30778D-662F-40C4-9890-8C670CA1EAE8}"/>
-    <hyperlink ref="D29" r:id="rId27" display="https://www.calendarlabs.com/holidays/us/independence-day.php" xr:uid="{06073432-295E-444E-ACC8-80B37C153678}"/>
-    <hyperlink ref="D30" r:id="rId28" display="https://www.calendarlabs.com/holidays/us/labor-day.php" xr:uid="{1964268F-92E6-4045-9079-34E1E87CB380}"/>
-    <hyperlink ref="D31" r:id="rId29" display="https://www.calendarlabs.com/holidays/us/columbus-day.php" xr:uid="{D6DD2C25-786E-468A-ABB6-81DC0D94C890}"/>
-    <hyperlink ref="D32" r:id="rId30" display="https://www.calendarlabs.com/holidays/us/halloween.php" xr:uid="{11D6FE7E-0957-4E48-8E08-BECA08E4426F}"/>
-    <hyperlink ref="D33" r:id="rId31" display="https://www.calendarlabs.com/holidays/us/veterans-day.php" xr:uid="{9DD762FD-F427-4270-B554-8E1FFAE3FBDD}"/>
-    <hyperlink ref="D34" r:id="rId32" display="https://www.calendarlabs.com/holidays/us/thanksgiving-day.php" xr:uid="{37666D02-44E6-4927-97B7-CEEB7BB2212A}"/>
-    <hyperlink ref="D35" r:id="rId33" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{930F418B-5698-4437-9D75-1CD5494F7E43}"/>
-    <hyperlink ref="D37" r:id="rId34" display="https://www.calendarlabs.com/holidays/us/new-years-day.php" xr:uid="{B3FB49CB-A9FE-40B1-A157-A4037286FDA3}"/>
-    <hyperlink ref="D38" r:id="rId35" display="https://www.calendarlabs.com/holidays/us/martin-luther-king-day.php" xr:uid="{E0BFEF64-1473-4DA0-BC6B-8E9AFF6DC5F8}"/>
-    <hyperlink ref="D39" r:id="rId36" display="https://www.calendarlabs.com/holidays/us/valentines-day.php" xr:uid="{7C66358F-AEC5-4F7F-9264-FEAA501D0645}"/>
-    <hyperlink ref="D40" r:id="rId37" display="https://www.calendarlabs.com/holidays/us/presidents-day.php" xr:uid="{90959777-163C-4E3D-95C4-AA6C2A6669E4}"/>
-    <hyperlink ref="D41" r:id="rId38" display="https://www.calendarlabs.com/holidays/us/good-friday.php" xr:uid="{D863EFE8-B704-4677-890B-453E191B8F23}"/>
-    <hyperlink ref="D42" r:id="rId39" display="https://www.calendarlabs.com/holidays/us/easter.php" xr:uid="{385B2704-4014-4FF1-8C79-24FCFD3357ED}"/>
-    <hyperlink ref="D43" r:id="rId40" display="https://www.calendarlabs.com/holidays/shared/mothers-day.php" xr:uid="{F3663FD5-03B6-436D-BDDA-3707E8A92BE3}"/>
-    <hyperlink ref="D44" r:id="rId41" display="https://www.calendarlabs.com/holidays/us/memorial-day.php" xr:uid="{7505FF12-9193-4759-AB0C-F93A963E70D0}"/>
-    <hyperlink ref="D45" r:id="rId42" display="https://www.calendarlabs.com/holidays/shared/fathers-day.php" xr:uid="{2353AA18-1A97-46C3-8456-C17B81C475C1}"/>
-    <hyperlink ref="D46" r:id="rId43" display="https://www.calendarlabs.com/holidays/us/independence-day.php" xr:uid="{E7297895-C5C9-49FA-B409-E36140009C6E}"/>
-    <hyperlink ref="D47" r:id="rId44" display="https://www.calendarlabs.com/holidays/us/independence-day.php" xr:uid="{1188041C-194A-40C4-9D6B-FB8515FC8FB2}"/>
-    <hyperlink ref="D48" r:id="rId45" display="https://www.calendarlabs.com/holidays/us/labor-day.php" xr:uid="{2C71894C-1C67-4E65-8897-BD918F51F8F9}"/>
-    <hyperlink ref="D49" r:id="rId46" display="https://www.calendarlabs.com/holidays/us/columbus-day.php" xr:uid="{44C388CB-6794-46B9-A268-8F3ECFFFE596}"/>
-    <hyperlink ref="D50" r:id="rId47" display="https://www.calendarlabs.com/holidays/us/halloween.php" xr:uid="{30B5DF01-F9E5-4CA7-8865-A72EDDA1C433}"/>
-    <hyperlink ref="D51" r:id="rId48" display="https://www.calendarlabs.com/holidays/us/veterans-day.php" xr:uid="{BD3FC977-70B8-4831-BFDE-0F0CAAFBB7F9}"/>
-    <hyperlink ref="D52" r:id="rId49" display="https://www.calendarlabs.com/holidays/us/thanksgiving-day.php" xr:uid="{B1CBA08F-C1EE-4389-8C20-A5834740A682}"/>
-    <hyperlink ref="D53" r:id="rId50" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{274449CB-896F-4176-AB4C-52215BB216D9}"/>
-    <hyperlink ref="D55" r:id="rId51" display="https://www.calendarlabs.com/holidays/us/new-years-day.php" xr:uid="{DF935B43-D5B8-4364-8AD1-9A137D9F3292}"/>
-    <hyperlink ref="D56" r:id="rId52" display="https://www.calendarlabs.com/holidays/us/martin-luther-king-day.php" xr:uid="{43D6B860-4C87-41CE-A7F2-7E7B294A6185}"/>
-    <hyperlink ref="D57" r:id="rId53" display="https://www.calendarlabs.com/holidays/us/valentines-day.php" xr:uid="{ED60D794-A320-4039-842F-C9AB2CF45653}"/>
-    <hyperlink ref="D58" r:id="rId54" display="https://www.calendarlabs.com/holidays/us/presidents-day.php" xr:uid="{E0CF33CD-9093-4E10-B9D2-E29F8D81712D}"/>
-    <hyperlink ref="D59" r:id="rId55" display="https://www.calendarlabs.com/holidays/us/good-friday.php" xr:uid="{49E63F02-2552-46B3-A75C-68CC4C19D821}"/>
-    <hyperlink ref="D60" r:id="rId56" display="https://www.calendarlabs.com/holidays/us/easter.php" xr:uid="{316FB145-2F60-46DB-B5D3-A70D7E7F6F86}"/>
-    <hyperlink ref="D61" r:id="rId57" display="https://www.calendarlabs.com/holidays/shared/mothers-day.php" xr:uid="{0A1E1F0E-4048-42D9-9A53-F292BCC834CA}"/>
-    <hyperlink ref="D62" r:id="rId58" display="https://www.calendarlabs.com/holidays/us/memorial-day.php" xr:uid="{F1467419-7A47-4878-BFD2-222EFC50601F}"/>
-    <hyperlink ref="D63" r:id="rId59" display="https://www.calendarlabs.com/holidays/shared/fathers-day.php" xr:uid="{AD77F1CF-2CDE-4D0A-8DD4-CAF5E5CBEA94}"/>
-    <hyperlink ref="D64" r:id="rId60" display="https://www.calendarlabs.com/holidays/us/independence-day.php" xr:uid="{208D944C-D591-4658-B817-567543C67BEE}"/>
-    <hyperlink ref="D65" r:id="rId61" display="https://www.calendarlabs.com/holidays/us/independence-day.php" xr:uid="{32C40836-F7AE-403A-AA2B-A24297681E50}"/>
-    <hyperlink ref="D66" r:id="rId62" display="https://www.calendarlabs.com/holidays/us/labor-day.php" xr:uid="{D20B573B-4B5B-481E-9FCD-40B4159B7586}"/>
-    <hyperlink ref="D67" r:id="rId63" display="https://www.calendarlabs.com/holidays/us/columbus-day.php" xr:uid="{D2B1FBC8-D939-4D6C-86FB-1B5D3DA9685B}"/>
-    <hyperlink ref="D68" r:id="rId64" display="https://www.calendarlabs.com/holidays/us/halloween.php" xr:uid="{78E4953E-4249-4F49-AE93-E523A881C45F}"/>
-    <hyperlink ref="D69" r:id="rId65" display="https://www.calendarlabs.com/holidays/us/veterans-day.php" xr:uid="{22784B30-F8C9-4354-89A4-B65A45D4BD51}"/>
-    <hyperlink ref="D70" r:id="rId66" display="https://www.calendarlabs.com/holidays/us/thanksgiving-day.php" xr:uid="{83D8B65D-3448-41CE-8CA0-D693C46E7EA1}"/>
-    <hyperlink ref="D71" r:id="rId67" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{2E704FE0-6969-48A4-86BB-1C196171B1F5}"/>
+    <hyperlink ref="D21" r:id="rId18" display="https://www.calendarlabs.com/holidays/us/new-years-day.php" xr:uid="{0D0A3B27-3D34-4C19-B07D-9C098EEED4F4}"/>
+    <hyperlink ref="D22" r:id="rId19" display="https://www.calendarlabs.com/holidays/us/martin-luther-king-day.php" xr:uid="{4077BA1B-E655-4EC7-BD39-841A949F73AC}"/>
+    <hyperlink ref="D23" r:id="rId20" display="https://www.calendarlabs.com/holidays/us/valentines-day.php" xr:uid="{5AEF472E-5A71-4AD3-920F-81BF657457B1}"/>
+    <hyperlink ref="D24" r:id="rId21" display="https://www.calendarlabs.com/holidays/us/presidents-day.php" xr:uid="{CDFA5CE1-09BF-45C4-A38D-F7243A4DA09F}"/>
+    <hyperlink ref="D25" r:id="rId22" display="https://www.calendarlabs.com/holidays/us/good-friday.php" xr:uid="{72D2E1E7-DDAE-4B2B-8EA6-143FC11F336D}"/>
+    <hyperlink ref="D26" r:id="rId23" display="https://www.calendarlabs.com/holidays/us/easter.php" xr:uid="{ABB7BC9D-62D8-419B-A8FD-47956F4941B2}"/>
+    <hyperlink ref="D27" r:id="rId24" display="https://www.calendarlabs.com/holidays/shared/mothers-day.php" xr:uid="{E52E46E1-B1BA-4373-B2D3-4F4D2EAF98B7}"/>
+    <hyperlink ref="D28" r:id="rId25" display="https://www.calendarlabs.com/holidays/us/memorial-day.php" xr:uid="{F1D41D0A-5D96-4868-9E86-2DF5395D14A8}"/>
+    <hyperlink ref="D29" r:id="rId26" display="https://www.calendarlabs.com/holidays/shared/fathers-day.php" xr:uid="{8F30778D-662F-40C4-9890-8C670CA1EAE8}"/>
+    <hyperlink ref="D30" r:id="rId27" display="https://www.calendarlabs.com/holidays/us/independence-day.php" xr:uid="{06073432-295E-444E-ACC8-80B37C153678}"/>
+    <hyperlink ref="D31" r:id="rId28" display="https://www.calendarlabs.com/holidays/us/labor-day.php" xr:uid="{1964268F-92E6-4045-9079-34E1E87CB380}"/>
+    <hyperlink ref="D32" r:id="rId29" display="https://www.calendarlabs.com/holidays/us/columbus-day.php" xr:uid="{D6DD2C25-786E-468A-ABB6-81DC0D94C890}"/>
+    <hyperlink ref="D33" r:id="rId30" display="https://www.calendarlabs.com/holidays/us/halloween.php" xr:uid="{11D6FE7E-0957-4E48-8E08-BECA08E4426F}"/>
+    <hyperlink ref="D34" r:id="rId31" display="https://www.calendarlabs.com/holidays/us/veterans-day.php" xr:uid="{9DD762FD-F427-4270-B554-8E1FFAE3FBDD}"/>
+    <hyperlink ref="D35" r:id="rId32" display="https://www.calendarlabs.com/holidays/us/thanksgiving-day.php" xr:uid="{37666D02-44E6-4927-97B7-CEEB7BB2212A}"/>
+    <hyperlink ref="D36" r:id="rId33" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{930F418B-5698-4437-9D75-1CD5494F7E43}"/>
+    <hyperlink ref="D39" r:id="rId34" display="https://www.calendarlabs.com/holidays/us/new-years-day.php" xr:uid="{B3FB49CB-A9FE-40B1-A157-A4037286FDA3}"/>
+    <hyperlink ref="D40" r:id="rId35" display="https://www.calendarlabs.com/holidays/us/martin-luther-king-day.php" xr:uid="{E0BFEF64-1473-4DA0-BC6B-8E9AFF6DC5F8}"/>
+    <hyperlink ref="D41" r:id="rId36" display="https://www.calendarlabs.com/holidays/us/valentines-day.php" xr:uid="{7C66358F-AEC5-4F7F-9264-FEAA501D0645}"/>
+    <hyperlink ref="D42" r:id="rId37" display="https://www.calendarlabs.com/holidays/us/presidents-day.php" xr:uid="{90959777-163C-4E3D-95C4-AA6C2A6669E4}"/>
+    <hyperlink ref="D43" r:id="rId38" display="https://www.calendarlabs.com/holidays/us/good-friday.php" xr:uid="{D863EFE8-B704-4677-890B-453E191B8F23}"/>
+    <hyperlink ref="D44" r:id="rId39" display="https://www.calendarlabs.com/holidays/us/easter.php" xr:uid="{385B2704-4014-4FF1-8C79-24FCFD3357ED}"/>
+    <hyperlink ref="D45" r:id="rId40" display="https://www.calendarlabs.com/holidays/shared/mothers-day.php" xr:uid="{F3663FD5-03B6-436D-BDDA-3707E8A92BE3}"/>
+    <hyperlink ref="D46" r:id="rId41" display="https://www.calendarlabs.com/holidays/us/memorial-day.php" xr:uid="{7505FF12-9193-4759-AB0C-F93A963E70D0}"/>
+    <hyperlink ref="D47" r:id="rId42" display="https://www.calendarlabs.com/holidays/shared/fathers-day.php" xr:uid="{2353AA18-1A97-46C3-8456-C17B81C475C1}"/>
+    <hyperlink ref="D48" r:id="rId43" display="https://www.calendarlabs.com/holidays/us/independence-day.php" xr:uid="{E7297895-C5C9-49FA-B409-E36140009C6E}"/>
+    <hyperlink ref="D49" r:id="rId44" display="https://www.calendarlabs.com/holidays/us/independence-day.php" xr:uid="{1188041C-194A-40C4-9D6B-FB8515FC8FB2}"/>
+    <hyperlink ref="D50" r:id="rId45" display="https://www.calendarlabs.com/holidays/us/labor-day.php" xr:uid="{2C71894C-1C67-4E65-8897-BD918F51F8F9}"/>
+    <hyperlink ref="D51" r:id="rId46" display="https://www.calendarlabs.com/holidays/us/columbus-day.php" xr:uid="{44C388CB-6794-46B9-A268-8F3ECFFFE596}"/>
+    <hyperlink ref="D52" r:id="rId47" display="https://www.calendarlabs.com/holidays/us/halloween.php" xr:uid="{30B5DF01-F9E5-4CA7-8865-A72EDDA1C433}"/>
+    <hyperlink ref="D53" r:id="rId48" display="https://www.calendarlabs.com/holidays/us/veterans-day.php" xr:uid="{BD3FC977-70B8-4831-BFDE-0F0CAAFBB7F9}"/>
+    <hyperlink ref="D54" r:id="rId49" display="https://www.calendarlabs.com/holidays/us/thanksgiving-day.php" xr:uid="{B1CBA08F-C1EE-4389-8C20-A5834740A682}"/>
+    <hyperlink ref="D55" r:id="rId50" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{274449CB-896F-4176-AB4C-52215BB216D9}"/>
+    <hyperlink ref="D58" r:id="rId51" display="https://www.calendarlabs.com/holidays/us/new-years-day.php" xr:uid="{DF935B43-D5B8-4364-8AD1-9A137D9F3292}"/>
+    <hyperlink ref="D59" r:id="rId52" display="https://www.calendarlabs.com/holidays/us/martin-luther-king-day.php" xr:uid="{43D6B860-4C87-41CE-A7F2-7E7B294A6185}"/>
+    <hyperlink ref="D60" r:id="rId53" display="https://www.calendarlabs.com/holidays/us/valentines-day.php" xr:uid="{ED60D794-A320-4039-842F-C9AB2CF45653}"/>
+    <hyperlink ref="D61" r:id="rId54" display="https://www.calendarlabs.com/holidays/us/presidents-day.php" xr:uid="{E0CF33CD-9093-4E10-B9D2-E29F8D81712D}"/>
+    <hyperlink ref="D62" r:id="rId55" display="https://www.calendarlabs.com/holidays/us/good-friday.php" xr:uid="{49E63F02-2552-46B3-A75C-68CC4C19D821}"/>
+    <hyperlink ref="D63" r:id="rId56" display="https://www.calendarlabs.com/holidays/us/easter.php" xr:uid="{316FB145-2F60-46DB-B5D3-A70D7E7F6F86}"/>
+    <hyperlink ref="D64" r:id="rId57" display="https://www.calendarlabs.com/holidays/shared/mothers-day.php" xr:uid="{0A1E1F0E-4048-42D9-9A53-F292BCC834CA}"/>
+    <hyperlink ref="D65" r:id="rId58" display="https://www.calendarlabs.com/holidays/us/memorial-day.php" xr:uid="{F1467419-7A47-4878-BFD2-222EFC50601F}"/>
+    <hyperlink ref="D66" r:id="rId59" display="https://www.calendarlabs.com/holidays/shared/fathers-day.php" xr:uid="{AD77F1CF-2CDE-4D0A-8DD4-CAF5E5CBEA94}"/>
+    <hyperlink ref="D67" r:id="rId60" display="https://www.calendarlabs.com/holidays/us/independence-day.php" xr:uid="{208D944C-D591-4658-B817-567543C67BEE}"/>
+    <hyperlink ref="D68" r:id="rId61" display="https://www.calendarlabs.com/holidays/us/independence-day.php" xr:uid="{32C40836-F7AE-403A-AA2B-A24297681E50}"/>
+    <hyperlink ref="D69" r:id="rId62" display="https://www.calendarlabs.com/holidays/us/labor-day.php" xr:uid="{D20B573B-4B5B-481E-9FCD-40B4159B7586}"/>
+    <hyperlink ref="D70" r:id="rId63" display="https://www.calendarlabs.com/holidays/us/columbus-day.php" xr:uid="{D2B1FBC8-D939-4D6C-86FB-1B5D3DA9685B}"/>
+    <hyperlink ref="D71" r:id="rId64" display="https://www.calendarlabs.com/holidays/us/halloween.php" xr:uid="{78E4953E-4249-4F49-AE93-E523A881C45F}"/>
+    <hyperlink ref="D72" r:id="rId65" display="https://www.calendarlabs.com/holidays/us/veterans-day.php" xr:uid="{22784B30-F8C9-4354-89A4-B65A45D4BD51}"/>
+    <hyperlink ref="D73" r:id="rId66" display="https://www.calendarlabs.com/holidays/us/thanksgiving-day.php" xr:uid="{83D8B65D-3448-41CE-8CA0-D693C46E7EA1}"/>
+    <hyperlink ref="D74" r:id="rId67" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{2E704FE0-6969-48A4-86BB-1C196171B1F5}"/>
+    <hyperlink ref="D19" r:id="rId68" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{62AAF6A2-7A0A-44E0-AC50-F714E7B4B1E1}"/>
+    <hyperlink ref="D37" r:id="rId69" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{39489978-49F0-479F-9275-774848076717}"/>
+    <hyperlink ref="D56" r:id="rId70" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{E9D66A22-AC7F-4942-B627-41CC4D3A60DE}"/>
+    <hyperlink ref="D75" r:id="rId71" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{1CEA009C-71E1-44D9-ABCD-3CEED4B9929A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId68"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId72"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB93130626BF8E4899FC05FDEF0CCD41" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ddc3e8a4b0144ff35620e4489b641c91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0967b7be50301903c78f9c39c6fd9af8">
     <xsd:element name="properties">
@@ -1564,15 +1623,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1580,13 +1630,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{435849B2-B1AD-4FC9-99EF-6B8217D6A796}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45C6FE90-2C7E-4A91-8C87-67C6FCA62795}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45C6FE90-2C7E-4A91-8C87-67C6FCA62795}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{435849B2-B1AD-4FC9-99EF-6B8217D6A796}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
dodati tipovi dana i potrosnja za prethodni dan u model
</commit_message>
<xml_diff>
--- a/Flask_Backend/rawTrainingData/holidays/Training Data_US Holidays 2018-2021.xlsx
+++ b/Flask_Backend/rawTrainingData/holidays/Training Data_US Holidays 2018-2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marko\Desktop\Training Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marko\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A42830-13BB-47E3-9627-C2296A379550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E6AAA7-DA10-459F-8958-E842BA5DC055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4B055610-134E-4B13-92E8-896F5ECCFBB2}"/>
+    <workbookView xWindow="3045" yWindow="2400" windowWidth="21600" windowHeight="11295" xr2:uid="{4B055610-134E-4B13-92E8-896F5ECCFBB2}"/>
   </bookViews>
   <sheets>
     <sheet name="US Holidays" sheetId="1" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0593F234-F7F3-4803-A580-A4FB13FCD7C2}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -819,7 +819,7 @@
       <c r="C19" s="15">
         <v>43465</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1011,7 +1011,7 @@
       <c r="C37" s="16">
         <v>43830</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1212,9 +1212,9 @@
         <v>19</v>
       </c>
       <c r="C56" s="14">
-        <v>44186</v>
-      </c>
-      <c r="D56" s="15" t="s">
+        <v>44196</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1417,7 +1417,7 @@
       <c r="C75" s="14">
         <v>44561</v>
       </c>
-      <c r="D75" s="15" t="s">
+      <c r="D75" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1490,13 +1490,9 @@
     <hyperlink ref="D72" r:id="rId65" display="https://www.calendarlabs.com/holidays/us/veterans-day.php" xr:uid="{22784B30-F8C9-4354-89A4-B65A45D4BD51}"/>
     <hyperlink ref="D73" r:id="rId66" display="https://www.calendarlabs.com/holidays/us/thanksgiving-day.php" xr:uid="{83D8B65D-3448-41CE-8CA0-D693C46E7EA1}"/>
     <hyperlink ref="D74" r:id="rId67" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{2E704FE0-6969-48A4-86BB-1C196171B1F5}"/>
-    <hyperlink ref="D19" r:id="rId68" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{62AAF6A2-7A0A-44E0-AC50-F714E7B4B1E1}"/>
-    <hyperlink ref="D37" r:id="rId69" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{39489978-49F0-479F-9275-774848076717}"/>
-    <hyperlink ref="D56" r:id="rId70" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{E9D66A22-AC7F-4942-B627-41CC4D3A60DE}"/>
-    <hyperlink ref="D75" r:id="rId71" display="https://www.calendarlabs.com/holidays/us/christmas.php" xr:uid="{1CEA009C-71E1-44D9-ABCD-3CEED4B9929A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId72"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId68"/>
 </worksheet>
 </file>
 

</xml_diff>